<commit_message>
Cleaned up, removing superfluous files, project builds with complete dependo curated set inc. aligns
</commit_message>
<xml_diff>
--- a/tabular/eve/epv_refseq_feature_locations.xlsx
+++ b/tabular/eve/epv_refseq_feature_locations.xlsx
@@ -3877,7 +3877,7 @@
   <dimension ref="A1:E1447"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:D11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4042,7 +4042,7 @@
         <v>1594</v>
       </c>
       <c r="D11" s="8">
-        <v>3728</v>
+        <v>3726</v>
       </c>
     </row>
     <row r="12" spans="1:4">

</xml_diff>